<commit_message>
Percentage change graph added
</commit_message>
<xml_diff>
--- a/Experimental data/BTP Graph.xlsx
+++ b/Experimental data/BTP Graph.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="15">
   <si>
     <t>Normal</t>
   </si>
@@ -49,12 +49,21 @@
   <si>
     <t>Apache</t>
   </si>
+  <si>
+    <t>CHANGES</t>
+  </si>
+  <si>
+    <t>% CHANGE</t>
+  </si>
+  <si>
+    <t>CHANGE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -65,6 +74,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,12 +94,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -254,11 +276,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1857719629"/>
-        <c:axId val="389112606"/>
+        <c:axId val="312517811"/>
+        <c:axId val="210653960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1857719629"/>
+        <c:axId val="312517811"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -310,10 +332,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="389112606"/>
+        <c:crossAx val="210653960"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="389112606"/>
+        <c:axId val="210653960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -388,7 +410,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1857719629"/>
+        <c:crossAx val="312517811"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -438,7 +460,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>Handshake time for various servers on different test</a:t>
+              <a:t>% Change in Packet RX time in various test</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -453,7 +475,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Handshake!$A$2</c:f>
+              <c:f>'Packet RX'!$A$27</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -468,12 +490,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Handshake!$B$1:$H$1</c:f>
+              <c:f>'Packet RX'!$B$26:$G$26</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Handshake!$B$2:$H$2</c:f>
+              <c:f>'Packet RX'!$B$27:$G$27</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -484,7 +506,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Handshake!$A$3</c:f>
+              <c:f>'Packet RX'!$A$28</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -499,12 +521,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Handshake!$B$1:$H$1</c:f>
+              <c:f>'Packet RX'!$B$26:$G$26</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Handshake!$B$3:$H$3</c:f>
+              <c:f>'Packet RX'!$B$28:$G$28</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -515,7 +537,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Handshake!$A$4</c:f>
+              <c:f>'Packet RX'!$A$29</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -530,12 +552,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Handshake!$B$1:$H$1</c:f>
+              <c:f>'Packet RX'!$B$26:$G$26</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Handshake!$B$4:$H$4</c:f>
+              <c:f>'Packet RX'!$B$29:$G$29</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -546,7 +568,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Handshake!$A$5</c:f>
+              <c:f>'Packet RX'!$A$30</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -561,22 +583,22 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Handshake!$B$1:$H$1</c:f>
+              <c:f>'Packet RX'!$B$26:$G$26</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Handshake!$B$5:$H$5</c:f>
+              <c:f>'Packet RX'!$B$30:$G$30</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="669737985"/>
-        <c:axId val="1042588518"/>
+        <c:axId val="784806124"/>
+        <c:axId val="1493513192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="669737985"/>
+        <c:axId val="784806124"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,10 +650,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1042588518"/>
+        <c:crossAx val="1493513192"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1042588518"/>
+        <c:axId val="1493513192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -706,7 +728,643 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="669737985"/>
+        <c:crossAx val="784806124"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Handshake time for various servers on different test</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Handshake!$A$2</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$B$1:$H$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$2:$H$2</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Handshake!$A$3</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$B$1:$H$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$3:$H$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Handshake!$A$4</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FBBC04"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$B$1:$H$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$4:$H$4</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Handshake!$A$5</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="34A853"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$B$1:$H$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$5:$H$5</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="980872953"/>
+        <c:axId val="262917185"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="980872953"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="262917185"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="262917185"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="980872953"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>% Change in Handshake time in various test</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Handshake!$A$28</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$B$27:$G$27</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$28:$G$28</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Handshake!$A$29</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$B$27:$G$27</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$29:$G$29</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Handshake!$A$30</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FBBC04"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$B$27:$G$27</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$30:$G$30</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Handshake!$A$31</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="34A853"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$B$27:$G$27</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$31:$G$31</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="172920750"/>
+        <c:axId val="1429790100"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="172920750"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1429790100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1429790100"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="172920750"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -736,12 +1394,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:ext cx="4600575" cy="2838450"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
@@ -759,17 +1417,12 @@
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
@@ -783,7 +1436,62 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3962400" cy="2457450"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1132,6 +1840,433 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8">
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1">
+        <v>177.846</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" ref="C11:C14" si="1"> ABS(B2 - C2)</f>
+        <v>6.827</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" ref="D11:D14" si="2"> ABS(B2 - D2)</f>
+        <v>7.231</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" ref="E11:E14" si="3"> ABS(B2 - E2)</f>
+        <v>4.404</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" ref="F11:F14" si="4"> ABS(B2 - F2)</f>
+        <v>12.66</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" ref="G11:G14" si="5"> ABS(B2 - G2)</f>
+        <v>9.181</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" ref="H11:H14" si="6"> ABS(B2 - H2)</f>
+        <v>15.683</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9.118</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="1"/>
+        <v>10.744</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="2"/>
+        <v>0.224</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="3"/>
+        <v>11.045</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="4"/>
+        <v>9.509</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="5"/>
+        <v>0.072</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="6"/>
+        <v>10.905</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1">
+        <v>159.575</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="1"/>
+        <v>4.509</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="2"/>
+        <v>11.506</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="3"/>
+        <v>21.005</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="4"/>
+        <v>5.561</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="5"/>
+        <v>0.009</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="6"/>
+        <v>20.286</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6.54</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.521</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.891</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="3"/>
+        <v>3.568</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="4"/>
+        <v>0.041</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="5"/>
+        <v>15.11</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="6"/>
+        <v>0.693</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1">
+        <v>177.846</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" ref="C20:C23" si="7"> (C11*100)/B11</f>
+        <v>3.838714393</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:D23" si="8"> (D11*100)/B11</f>
+        <v>4.06587722</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" ref="E20:E23" si="9"> (E11*100)/B11</f>
+        <v>2.47629972</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" ref="F20:F23" si="10"> (F11*100)/B11</f>
+        <v>7.118518269</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" ref="G20:G23" si="11"> (G11*100)/B11</f>
+        <v>5.162331455</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" ref="H20:H23" si="12"> (H11*100)/B11</f>
+        <v>8.818303476</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1">
+        <v>9.118</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="7"/>
+        <v>117.8328581</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="8"/>
+        <v>2.456679096</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="9"/>
+        <v>121.1340206</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="10"/>
+        <v>104.2882211</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="11"/>
+        <v>0.7896468524</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="12"/>
+        <v>119.5985962</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1">
+        <v>159.575</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="7"/>
+        <v>2.825630581</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="8"/>
+        <v>7.210402632</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="9"/>
+        <v>13.16308946</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="10"/>
+        <v>3.484881717</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="11"/>
+        <v>0.0056399812</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="12"/>
+        <v>12.71251762</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1">
+        <v>6.54</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="7"/>
+        <v>23.25688073</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="8"/>
+        <v>13.62385321</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="9"/>
+        <v>54.55657492</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="10"/>
+        <v>0.626911315</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="11"/>
+        <v>231.0397554</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="12"/>
+        <v>10.59633028</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="4">
+        <v>3.838714393</v>
+      </c>
+      <c r="C27" s="4">
+        <v>4.06587722</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2.47629972</v>
+      </c>
+      <c r="E27" s="4">
+        <v>7.118518269</v>
+      </c>
+      <c r="F27" s="4">
+        <v>5.162331455</v>
+      </c>
+      <c r="G27" s="4">
+        <v>8.818303476</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="4">
+        <v>117.8328581</v>
+      </c>
+      <c r="C28" s="4">
+        <v>2.456679096</v>
+      </c>
+      <c r="D28" s="4">
+        <v>121.1340206</v>
+      </c>
+      <c r="E28" s="4">
+        <v>104.2882211</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0.789646852</v>
+      </c>
+      <c r="G28" s="4">
+        <v>119.5985962</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="4">
+        <v>2.825630581</v>
+      </c>
+      <c r="C29" s="4">
+        <v>7.210402632</v>
+      </c>
+      <c r="D29" s="4">
+        <v>13.16308946</v>
+      </c>
+      <c r="E29" s="4">
+        <v>3.484881717</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0.005639981</v>
+      </c>
+      <c r="G29" s="4">
+        <v>12.71251762</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="4">
+        <v>23.25688073</v>
+      </c>
+      <c r="C30" s="4">
+        <v>13.62385321</v>
+      </c>
+      <c r="D30" s="4">
+        <v>54.55657492</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.626911315</v>
+      </c>
+      <c r="F30" s="4">
+        <v>231.0397554</v>
+      </c>
+      <c r="G30" s="4">
+        <v>10.59633028</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1283,6 +2418,433 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8">
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1">
+        <v>89.9</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" ref="C11:C14" si="1"> ABS(B2 - C2)</f>
+        <v>2.801</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" ref="D11:D14" si="2"> ABS(B2 - D2)</f>
+        <v>2.894</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" ref="E11:E14" si="3"> ABS(B2 - E2)</f>
+        <v>1.648</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" ref="F11:F14" si="4"> ABS(B2 - F2)</f>
+        <v>9.501</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" ref="G11:G14" si="5"> ABS(B2 - G2)</f>
+        <v>5.674</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" ref="H11:H14" si="6"> ABS(B2 - H2)</f>
+        <v>15.484</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>8.037</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="1"/>
+        <v>2.165</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="2"/>
+        <v>0.261</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="3"/>
+        <v>1.894</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="4"/>
+        <v>1.104</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="5"/>
+        <v>0.103</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="6"/>
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1">
+        <v>78.673</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="1"/>
+        <v>2.416</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="2"/>
+        <v>5.671</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="3"/>
+        <v>10.163</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="4"/>
+        <v>2.786</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="5"/>
+        <v>0.125</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="6"/>
+        <v>8.979</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3.283</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.078</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="2"/>
+        <v>1.475</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="3"/>
+        <v>0.987</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="4"/>
+        <v>0.726</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="5"/>
+        <v>0.205</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="6"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1">
+        <v>89.9</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" ref="C20:C23" si="7"> (C11*100)/B11</f>
+        <v>3.115684093</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:D23" si="8"> (D11*100)/B11</f>
+        <v>3.219132369</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" ref="E20:E23" si="9"> (E11*100)/B11</f>
+        <v>1.833147942</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" ref="F20:F23" si="10"> (F11*100)/B11</f>
+        <v>10.56840934</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" ref="G20:G23" si="11"> (G11*100)/B11</f>
+        <v>6.311457175</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" ref="H20:H23" si="12"> (H11*100)/B11</f>
+        <v>17.22358176</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8.037</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="7"/>
+        <v>26.93791216</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="8"/>
+        <v>3.247480403</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="9"/>
+        <v>23.56600722</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="10"/>
+        <v>13.73646883</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="11"/>
+        <v>1.281572726</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="12"/>
+        <v>20.65447306</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1">
+        <v>78.673</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="7"/>
+        <v>3.070939204</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="8"/>
+        <v>7.208317974</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="9"/>
+        <v>12.91802779</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="10"/>
+        <v>3.541240324</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="11"/>
+        <v>0.1588855135</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="12"/>
+        <v>11.4130642</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1">
+        <v>3.283</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="7"/>
+        <v>2.375875723</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="8"/>
+        <v>44.92841913</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="9"/>
+        <v>30.06396588</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="10"/>
+        <v>22.11392019</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="11"/>
+        <v>6.24428876</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="12"/>
+        <v>22.84495888</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="4">
+        <v>3.115684093</v>
+      </c>
+      <c r="C28" s="4">
+        <v>3.219132369</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1.833147942</v>
+      </c>
+      <c r="E28" s="4">
+        <v>10.56840934</v>
+      </c>
+      <c r="F28" s="4">
+        <v>6.311457175</v>
+      </c>
+      <c r="G28" s="4">
+        <v>17.22358176</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="4">
+        <v>26.93791216</v>
+      </c>
+      <c r="C29" s="4">
+        <v>3.247480403</v>
+      </c>
+      <c r="D29" s="4">
+        <v>23.56600722</v>
+      </c>
+      <c r="E29" s="4">
+        <v>13.73646883</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1.281572726</v>
+      </c>
+      <c r="G29" s="4">
+        <v>20.65447306</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="4">
+        <v>3.070939204</v>
+      </c>
+      <c r="C30" s="4">
+        <v>7.208317974</v>
+      </c>
+      <c r="D30" s="4">
+        <v>12.91802779</v>
+      </c>
+      <c r="E30" s="4">
+        <v>3.541240324</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0.158885514</v>
+      </c>
+      <c r="G30" s="4">
+        <v>11.4130642</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="4">
+        <v>2.375875723</v>
+      </c>
+      <c r="C31" s="4">
+        <v>44.92841913</v>
+      </c>
+      <c r="D31" s="4">
+        <v>30.06396588</v>
+      </c>
+      <c r="E31" s="4">
+        <v>22.11392019</v>
+      </c>
+      <c r="F31" s="4">
+        <v>6.24428876</v>
+      </c>
+      <c r="G31" s="4">
+        <v>22.84495888</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Graph added for average change
</commit_message>
<xml_diff>
--- a/Experimental data/BTP Graph.xlsx
+++ b/Experimental data/BTP Graph.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="16">
   <si>
     <t>Normal</t>
   </si>
@@ -56,6 +56,9 @@
     <t>% CHANGE</t>
   </si>
   <si>
+    <t>Average Percentage change</t>
+  </si>
+  <si>
     <t>CHANGE</t>
   </si>
 </sst>
@@ -94,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -110,6 +113,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -276,11 +280,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="312517811"/>
-        <c:axId val="210653960"/>
+        <c:axId val="1123896088"/>
+        <c:axId val="314894955"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="312517811"/>
+        <c:axId val="1123896088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -332,10 +336,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210653960"/>
+        <c:crossAx val="314894955"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210653960"/>
+        <c:axId val="314894955"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -410,7 +414,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312517811"/>
+        <c:crossAx val="1123896088"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -594,11 +598,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="784806124"/>
-        <c:axId val="1493513192"/>
+        <c:axId val="1203615094"/>
+        <c:axId val="953349889"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="784806124"/>
+        <c:axId val="1203615094"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -650,10 +654,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1493513192"/>
+        <c:crossAx val="953349889"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1493513192"/>
+        <c:axId val="953349889"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -728,7 +732,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="784806124"/>
+        <c:crossAx val="1203615094"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -778,7 +782,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>Handshake time for various servers on different test</a:t>
+              <a:t>Average Percentage change in Packet RX time</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -787,136 +791,38 @@
     </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
+      <c:barChart>
+        <c:barDir val="col"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Handshake!$A$2</c:f>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
-                <a:srgbClr val="4285F4"/>
+                <a:srgbClr val="000000"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Handshake!$B$1:$H$1</c:f>
+              <c:f>'Packet RX'!$A$35:$A$38</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Handshake!$B$2:$H$2</c:f>
+              <c:f>'Packet RX'!$B$35:$B$38</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Handshake!$A$3</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="EA4335"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Handshake!$B$1:$H$1</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Handshake!$B$3:$H$3</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Handshake!$A$4</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="FBBC04"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Handshake!$B$1:$H$1</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Handshake!$B$4:$H$4</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Handshake!$A$5</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="34A853"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Handshake!$B$1:$H$1</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Handshake!$B$5:$H$5</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="980872953"/>
-        <c:axId val="262917185"/>
-      </c:lineChart>
+        <c:axId val="1617777898"/>
+        <c:axId val="2123871248"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="980872953"/>
+        <c:axId val="1617777898"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,10 +874,328 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262917185"/>
+        <c:crossAx val="2123871248"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="262917185"/>
+        <c:axId val="2123871248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Average Percentage change</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1617777898"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Handshake time for various servers on different test</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Handshake!$A$2</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$B$1:$H$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$2:$H$2</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Handshake!$A$3</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$B$1:$H$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$3:$H$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Handshake!$A$4</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FBBC04"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$B$1:$H$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$4:$H$4</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Handshake!$A$5</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="34A853"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$B$1:$H$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$5:$H$5</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1287850403"/>
+        <c:axId val="2128867282"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1287850403"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2128867282"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2128867282"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1046,7 +1270,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="980872953"/>
+        <c:crossAx val="1287850403"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1072,7 +1296,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -1230,11 +1454,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="172920750"/>
-        <c:axId val="1429790100"/>
+        <c:axId val="279404645"/>
+        <c:axId val="2036904076"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="172920750"/>
+        <c:axId val="279404645"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,10 +1510,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1429790100"/>
+        <c:crossAx val="2036904076"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1429790100"/>
+        <c:axId val="2036904076"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1364,7 +1588,227 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172920750"/>
+        <c:crossAx val="279404645"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Average Percentage change in handshake time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Handshake!$A$37:$A$40</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Handshake!$B$37:$B$40</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1772066113"/>
+        <c:axId val="1773908492"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1772066113"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1773908492"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1773908492"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Average Percentage change</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1772066113"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1419,12 +1863,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:ext cx="4600575" cy="2838450"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
@@ -1437,6 +1881,31 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1628775</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1457,7 +1926,7 @@
     <xdr:ext cx="3962400" cy="2457450"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1482,7 +1951,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
+        <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1492,6 +1961,31 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2267,6 +2761,47 @@
         <v>10.59633028</v>
       </c>
     </row>
+    <row r="34">
+      <c r="B34" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="5">
+        <f t="shared" ref="B35:B38" si="13"> AVERAGE(C11:H11)*100/B11</f>
+        <v>5.246674089</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="5">
+        <f t="shared" si="13"/>
+        <v>77.68333699</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="5">
+        <f t="shared" si="13"/>
+        <v>6.567026999</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="5">
+        <f t="shared" si="13"/>
+        <v>55.61671764</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2420,7 +2955,7 @@
     </row>
     <row r="8">
       <c r="E8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
@@ -2845,6 +3380,53 @@
         <v>22.84495888</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="5">
+        <f t="shared" ref="B37:B40" si="13"> AVERAGE(C11:H11)*100/B11</f>
+        <v>7.045235447</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="5">
+        <f t="shared" si="13"/>
+        <v>14.90398573</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="5">
+        <f t="shared" si="13"/>
+        <v>6.385079167</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="5">
+        <f t="shared" si="13"/>
+        <v>21.42857143</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>